<commit_message>
added exploratory data analysis
</commit_message>
<xml_diff>
--- a/Manufacturing/naics.xlsx
+++ b/Manufacturing/naics.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steve\Documents\QMSS\CDUP\Commodity Flows Survey\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Schinria/cdup-manufacturing/Manufacturing/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6816"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24700" windowHeight="15500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -205,31 +208,31 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -238,10 +241,10 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -249,25 +252,25 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -364,9 +367,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -399,9 +402,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -587,9 +590,12 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="32.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>45</v>
       </c>
@@ -597,7 +603,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="43.5" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" ht="46" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>212</v>
       </c>
@@ -605,7 +611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>311</v>
       </c>
@@ -613,7 +619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" ht="90" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>312</v>
       </c>
@@ -621,7 +627,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>313</v>
       </c>
@@ -629,7 +635,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>314</v>
       </c>
@@ -637,7 +643,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>315</v>
       </c>
@@ -645,7 +651,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:2" ht="75" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>316</v>
       </c>
@@ -653,7 +659,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>321</v>
       </c>
@@ -661,7 +667,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>322</v>
       </c>
@@ -669,7 +675,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:2" ht="75" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>323</v>
       </c>
@@ -677,7 +683,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:2" ht="90" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>324</v>
       </c>
@@ -685,7 +691,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:2" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>325</v>
       </c>
@@ -693,7 +699,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:2" ht="90" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>326</v>
       </c>
@@ -701,7 +707,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:2" ht="75" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>327</v>
       </c>
@@ -709,7 +715,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:2" ht="60" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>331</v>
       </c>
@@ -717,7 +723,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:2" ht="75" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <v>332</v>
       </c>
@@ -725,7 +731,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:2" ht="60" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>333</v>
       </c>
@@ -733,7 +739,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:2" ht="90" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>334</v>
       </c>
@@ -741,7 +747,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:2" ht="135" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
         <v>335</v>
       </c>
@@ -749,7 +755,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:2" ht="90" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <v>336</v>
       </c>
@@ -757,7 +763,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:2" ht="90" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
         <v>337</v>
       </c>
@@ -765,7 +771,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:2" ht="60" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
         <v>339</v>
       </c>
@@ -773,7 +779,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:2" ht="90" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
         <v>4231</v>
       </c>
@@ -781,7 +787,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:2" ht="90" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
         <v>4232</v>
       </c>
@@ -789,7 +795,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:2" ht="120" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
         <v>4233</v>
       </c>
@@ -797,7 +803,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:2" ht="75" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
         <v>4234</v>
       </c>
@@ -805,7 +811,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:2" ht="120" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
         <v>4235</v>
       </c>
@@ -813,7 +819,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:2" ht="105" x14ac:dyDescent="0.2">
       <c r="A29" s="5">
         <v>4236</v>
       </c>
@@ -821,7 +827,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:2" ht="90" x14ac:dyDescent="0.2">
       <c r="A30" s="5">
         <v>4237</v>
       </c>
@@ -829,7 +835,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:2" ht="120" x14ac:dyDescent="0.2">
       <c r="A31" s="5">
         <v>4238</v>
       </c>
@@ -837,7 +843,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:2" ht="105" x14ac:dyDescent="0.2">
       <c r="A32" s="5">
         <v>4239</v>
       </c>
@@ -845,7 +851,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:2" ht="90" x14ac:dyDescent="0.2">
       <c r="A33" s="5">
         <v>4241</v>
       </c>
@@ -853,7 +859,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:2" ht="90" x14ac:dyDescent="0.2">
       <c r="A34" s="5">
         <v>4242</v>
       </c>
@@ -861,7 +867,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:2" ht="120" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
         <v>4243</v>
       </c>
@@ -869,7 +875,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:2" ht="105" x14ac:dyDescent="0.2">
       <c r="A36" s="5">
         <v>4244</v>
       </c>
@@ -877,7 +883,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:2" ht="105" x14ac:dyDescent="0.2">
       <c r="A37" s="5">
         <v>4245</v>
       </c>
@@ -885,7 +891,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:2" ht="90" x14ac:dyDescent="0.2">
       <c r="A38" s="5">
         <v>4246</v>
       </c>
@@ -893,7 +899,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:2" ht="120" x14ac:dyDescent="0.2">
       <c r="A39" s="5">
         <v>4247</v>
       </c>
@@ -901,7 +907,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:2" ht="120" x14ac:dyDescent="0.2">
       <c r="A40" s="5">
         <v>4248</v>
       </c>
@@ -909,7 +915,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:2" ht="105" x14ac:dyDescent="0.2">
       <c r="A41" s="5">
         <v>4249</v>
       </c>
@@ -917,7 +923,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:2" ht="75" x14ac:dyDescent="0.2">
       <c r="A42" s="5">
         <v>4541</v>
       </c>
@@ -925,7 +931,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:2" ht="60" x14ac:dyDescent="0.2">
       <c r="A43" s="5">
         <v>45431</v>
       </c>
@@ -933,7 +939,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:2" ht="75" x14ac:dyDescent="0.2">
       <c r="A44" s="5">
         <v>4931</v>
       </c>
@@ -941,7 +947,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:2" ht="90" x14ac:dyDescent="0.2">
       <c r="A45" s="5">
         <v>5111</v>
       </c>
@@ -949,7 +955,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:2" ht="105" x14ac:dyDescent="0.2">
       <c r="A46" s="7">
         <v>551114</v>
       </c>

</xml_diff>